<commit_message>
fixed std error on after_26th els
</commit_message>
<xml_diff>
--- a/data_after_26.xlsx
+++ b/data_after_26.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="40">
   <si>
     <t>age</t>
   </si>
@@ -111,15 +111,6 @@
     <t>Stderror=stddev/sqrt(samplesize)</t>
   </si>
   <si>
-    <t>ribbin_errors</t>
-  </si>
-  <si>
-    <t>ribbon_rating</t>
-  </si>
-  <si>
-    <t>cmap_rating</t>
-  </si>
-  <si>
     <t>Ribbon (Different Parent )</t>
   </si>
   <si>
@@ -136,6 +127,18 @@
   </si>
   <si>
     <t>Command Map</t>
+  </si>
+  <si>
+    <t>Errors on Ribbon</t>
+  </si>
+  <si>
+    <t>Errors on CommandMaps</t>
+  </si>
+  <si>
+    <t>Rating for Ribbon</t>
+  </si>
+  <si>
+    <t>Rating for CommandMaps</t>
   </si>
 </sst>
 </file>
@@ -253,6 +256,30 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Mean Time</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> per Trial</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -310,28 +337,28 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="8"/>
                   <c:pt idx="0">
-                    <c:v>186.757619559216</c:v>
+                    <c:v>216.1571319143048</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>175.9348925357078</c:v>
+                    <c:v>203.6306837917896</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>184.5159304491839</c:v>
+                    <c:v>213.5625545695533</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>169.6732103334294</c:v>
+                    <c:v>196.3832832894813</c:v>
                   </c:pt>
                   <c:pt idx="5">
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>426.688618857044</c:v>
+                    <c:v>493.8582334166575</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>356.2569518062242</c:v>
+                    <c:v>412.339165109936</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -343,28 +370,28 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="8"/>
                   <c:pt idx="0">
-                    <c:v>186.757619559216</c:v>
+                    <c:v>216.1571319143048</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>175.9348925357078</c:v>
+                    <c:v>203.6306837917896</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>184.5159304491839</c:v>
+                    <c:v>213.5625545695533</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>169.6732103334294</c:v>
+                    <c:v>196.3832832894813</c:v>
                   </c:pt>
                   <c:pt idx="5">
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>426.688618857044</c:v>
+                    <c:v>493.8582334166575</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>356.2569518062242</c:v>
+                    <c:v>412.339165109936</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -433,11 +460,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2121433752"/>
-        <c:axId val="2121430760"/>
+        <c:axId val="2145706600"/>
+        <c:axId val="2146142744"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2121433752"/>
+        <c:axId val="2145706600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -446,7 +473,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121430760"/>
+        <c:crossAx val="2146142744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -454,7 +481,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2121430760"/>
+        <c:axId val="2146142744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -465,7 +492,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121433752"/>
+        <c:crossAx val="2145706600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -496,6 +523,30 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Mean Errors</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> after 72 Trial Experiment</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -533,10 +584,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>0.129706318355906</c:v>
+                    <c:v>0.150124775809142</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.098487093977041</c:v>
+                    <c:v>0.113990999750892</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -548,10 +599,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>0.129706318355906</c:v>
+                    <c:v>0.150124775809142</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.098487093977041</c:v>
+                    <c:v>0.113990999750892</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -563,10 +614,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>ribbin_errors</c:v>
+                  <c:v>Errors on Ribbon</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>cmap_errors</c:v>
+                  <c:v>Errors on CommandMaps</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -596,11 +647,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2121402248"/>
-        <c:axId val="2121399256"/>
+        <c:axId val="2146399096"/>
+        <c:axId val="2145937160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2121402248"/>
+        <c:axId val="2146399096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -609,7 +660,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121399256"/>
+        <c:crossAx val="2145937160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -617,7 +668,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2121399256"/>
+        <c:axId val="2145937160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -628,7 +679,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121402248"/>
+        <c:crossAx val="2146399096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -664,6 +715,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Mean Rating</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -701,10 +771,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>0.0976009787961143</c:v>
+                    <c:v>0.112965391711408</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.119193786636154</c:v>
+                    <c:v>0.13795735414751</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -716,10 +786,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>0.0976009787961143</c:v>
+                    <c:v>0.112965391711408</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.119193786636154</c:v>
+                    <c:v>0.13795735414751</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -731,10 +801,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>ribbon_rating</c:v>
+                  <c:v>Rating for Ribbon</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>cmap_rating</c:v>
+                  <c:v>Rating for CommandMaps</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -764,11 +834,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2121372232"/>
-        <c:axId val="2121369240"/>
+        <c:axId val="2146023512"/>
+        <c:axId val="2146018120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2121372232"/>
+        <c:axId val="2146023512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -777,7 +847,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121369240"/>
+        <c:crossAx val="2146018120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -785,7 +855,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2121369240"/>
+        <c:axId val="2146018120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -796,7 +866,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121372232"/>
+        <c:crossAx val="2146023512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -853,15 +923,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
+      <xdr:colOff>177800</xdr:colOff>
       <xdr:row>65</xdr:row>
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>79</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -883,15 +953,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>508000</xdr:colOff>
+      <xdr:colOff>165100</xdr:colOff>
       <xdr:row>82</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>96</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1237,8 +1307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="L58" sqref="L58"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="T73" sqref="T73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4032,34 +4102,34 @@
     </row>
     <row r="58" spans="1:17">
       <c r="B58" t="s">
+        <v>34</v>
+      </c>
+      <c r="C58" t="s">
+        <v>35</v>
+      </c>
+      <c r="E58" t="s">
+        <v>30</v>
+      </c>
+      <c r="F58" t="s">
+        <v>31</v>
+      </c>
+      <c r="H58" t="s">
+        <v>32</v>
+      </c>
+      <c r="I58" t="s">
+        <v>33</v>
+      </c>
+      <c r="L58" t="s">
+        <v>36</v>
+      </c>
+      <c r="M58" t="s">
         <v>37</v>
       </c>
-      <c r="C58" t="s">
+      <c r="N58" t="s">
         <v>38</v>
       </c>
-      <c r="E58" t="s">
-        <v>33</v>
-      </c>
-      <c r="F58" t="s">
-        <v>34</v>
-      </c>
-      <c r="H58" t="s">
-        <v>35</v>
-      </c>
-      <c r="I58" t="s">
-        <v>36</v>
-      </c>
-      <c r="L58" t="s">
-        <v>30</v>
-      </c>
-      <c r="M58" t="s">
-        <v>15</v>
-      </c>
-      <c r="N58" t="s">
-        <v>31</v>
-      </c>
       <c r="O58" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="59" spans="1:17">
@@ -4157,52 +4227,52 @@
         <v>29</v>
       </c>
       <c r="B61">
-        <f>B60/(71 ^ 0.5)</f>
-        <v>186.75761955921595</v>
+        <f>B60/(53 ^ 0.5)</f>
+        <v>216.15713191430484</v>
       </c>
       <c r="C61">
-        <f t="shared" ref="C61:O61" si="0">C60/(71 ^ 0.5)</f>
-        <v>175.93489253570777</v>
+        <f>C60/(53 ^ 0.5)</f>
+        <v>203.63068379178955</v>
       </c>
       <c r="D61">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C61:O61" si="0">D60/(71 ^ 0.5)</f>
         <v>0</v>
       </c>
       <c r="E61">
-        <f t="shared" si="0"/>
-        <v>184.51593044918388</v>
+        <f>E60/(53 ^ 0.5)</f>
+        <v>213.56255456955333</v>
       </c>
       <c r="F61">
-        <f t="shared" si="0"/>
-        <v>169.67321033342938</v>
+        <f>F60/(53 ^ 0.5)</f>
+        <v>196.38328328948134</v>
       </c>
       <c r="G61">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H61">
-        <f t="shared" si="0"/>
-        <v>426.68861885704399</v>
+        <f>H60/(53 ^ 0.5)</f>
+        <v>493.85823341665753</v>
       </c>
       <c r="I61">
-        <f t="shared" si="0"/>
-        <v>356.25695180622421</v>
+        <f>I60/(53 ^ 0.5)</f>
+        <v>412.339165109936</v>
       </c>
       <c r="L61">
-        <f t="shared" si="0"/>
-        <v>0.12970631835590588</v>
+        <f>L60/(53 ^ 0.5)</f>
+        <v>0.15012477580914221</v>
       </c>
       <c r="M61">
-        <f t="shared" si="0"/>
-        <v>9.8487093977041057E-2</v>
+        <f>M60/(53 ^ 0.5)</f>
+        <v>0.11399099975089219</v>
       </c>
       <c r="N61">
-        <f t="shared" si="0"/>
-        <v>9.7600978796114374E-2</v>
+        <f>N60/(53 ^ 0.5)</f>
+        <v>0.11296539171140811</v>
       </c>
       <c r="O61">
-        <f t="shared" si="0"/>
-        <v>0.11919378663615404</v>
+        <f>O60/(53 ^ 0.5)</f>
+        <v>0.13795735414750979</v>
       </c>
     </row>
   </sheetData>

</xml_diff>